<commit_message>
I CANT FIX PAGINATION, the rest is fixed tho :)
</commit_message>
<xml_diff>
--- a/Intern Documentation/DnDUnderground Planning.xlsx
+++ b/Intern Documentation/DnDUnderground Planning.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94187846-7067-4239-BBC7-87438063BD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4135D2-8C00-49E1-A92F-4068B856E818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2391,8 +2391,8 @@
   </sheetPr>
   <dimension ref="A1:BO109"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A17" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3192,7 +3192,7 @@
       <c r="D10" s="46"/>
       <c r="E10" s="85">
         <f t="shared" ref="E10:E108" ca="1" si="4">TODAY()</f>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="F10" s="47"/>
       <c r="H10" s="48"/>
@@ -6643,7 +6643,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="56" t="s">
         <v>44</v>
@@ -6886,7 +6886,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
       <c r="B26" s="56" t="s">
         <v>46</v>
@@ -7129,7 +7129,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="56" t="s">
         <v>43</v>
@@ -7372,7 +7372,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="56" t="s">
         <v>38</v>
@@ -7867,7 +7867,7 @@
         <v>10</v>
       </c>
       <c r="D30" s="57">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E30" s="87">
         <v>45363</v>
@@ -8110,7 +8110,7 @@
         <v>10</v>
       </c>
       <c r="D31" s="57">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E31" s="87">
         <v>45364</v>
@@ -8353,7 +8353,7 @@
         <v>10</v>
       </c>
       <c r="D32" s="57">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E32" s="87">
         <v>45362</v>
@@ -8596,7 +8596,7 @@
         <v>10</v>
       </c>
       <c r="D33" s="57">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E33" s="87">
         <v>45363</v>
@@ -23596,7 +23596,7 @@
       <c r="D95" s="68"/>
       <c r="E95" s="90">
         <f t="shared" ca="1" si="4"/>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="F95" s="69"/>
       <c r="G95" s="53"/>
@@ -23836,7 +23836,7 @@
       </c>
       <c r="E96" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="F96" s="58">
         <v>4</v>
@@ -24078,7 +24078,7 @@
       </c>
       <c r="E97" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="F97" s="58">
         <v>14</v>
@@ -24320,7 +24320,7 @@
       </c>
       <c r="E98" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="F98" s="58">
         <v>6</v>
@@ -24562,7 +24562,7 @@
       </c>
       <c r="E99" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="F99" s="58">
         <v>3</v>
@@ -24804,7 +24804,7 @@
       </c>
       <c r="E100" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="F100" s="58">
         <v>19</v>
@@ -25044,7 +25044,7 @@
       <c r="D101" s="72"/>
       <c r="E101" s="91">
         <f t="shared" ca="1" si="4"/>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="F101" s="73"/>
       <c r="G101" s="53"/>
@@ -25284,7 +25284,7 @@
       </c>
       <c r="E102" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="F102" s="58">
         <v>15</v>
@@ -25526,7 +25526,7 @@
       </c>
       <c r="E103" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="F103" s="58">
         <v>5</v>
@@ -25768,7 +25768,7 @@
       </c>
       <c r="E104" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="F104" s="58">
         <v>1</v>
@@ -26010,7 +26010,7 @@
       </c>
       <c r="E105" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="F105" s="58"/>
       <c r="G105" s="53"/>
@@ -26250,7 +26250,7 @@
       </c>
       <c r="E106" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="F106" s="58"/>
       <c r="G106" s="53"/>
@@ -26486,7 +26486,7 @@
       <c r="D107" s="57"/>
       <c r="E107" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="F107" s="58"/>
       <c r="G107" s="53"/>
@@ -26725,7 +26725,7 @@
       <c r="D108" s="21"/>
       <c r="E108" s="92">
         <f t="shared" ca="1" si="4"/>
-        <v>45358</v>
+        <v>45364</v>
       </c>
       <c r="F108" s="76"/>
       <c r="G108" s="53"/>
@@ -27173,6 +27173,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -27472,7 +27481,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
@@ -27492,16 +27501,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16A2ABA2-2AE7-458F-84A6-54746C92ACFB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CDF409-87B8-4BD3-A7A0-FA31B09DB512}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27522,7 +27530,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D0FD509-FAA6-490F-8E99-57602ADB216E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -27534,14 +27542,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16A2ABA2-2AE7-458F-84A6-54746C92ACFB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
filtering has been completed /monsters page FULLY DONE || TODO add filtering to Spells page (might remake this page)
</commit_message>
<xml_diff>
--- a/Intern Documentation/DnDUnderground Planning.xlsx
+++ b/Intern Documentation/DnDUnderground Planning.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4135D2-8C00-49E1-A92F-4068B856E818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68502489-BB86-49FF-85BF-3777057693BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1184,162 +1184,20 @@
   <dxfs count="34">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color auto="1"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
       <border>
         <left/>
         <right/>
         <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1452,6 +1310,92 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -1491,38 +1435,94 @@
     </dxf>
     <dxf>
       <font>
-        <color auto="1"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1927,7 +1927,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{876EA49D-634E-482B-8173-880F7B761E2C}" name="Milestones43524" displayName="Milestones43524" ref="B9:F108" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{876EA49D-634E-482B-8173-880F7B761E2C}" name="Milestones43524" displayName="Milestones43524" ref="B9:F108" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="B9:F108" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1936,13 +1936,13 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0971B905-713A-4980-8BBC-DF959C2E61F9}" name="Milestone description" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{4492A0B8-068F-4002-9E8D-E1F5FED367F0}" name="Category" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{47C54592-75B0-4C70-BBF8-0F40483670E9}" name="Progress" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{663FB5E0-7616-4EA5-B56A-FF069E2E07D7}" name="Start" dataDxfId="1" dataCellStyle="Date">
+    <tableColumn id="1" xr3:uid="{0971B905-713A-4980-8BBC-DF959C2E61F9}" name="Milestone description" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{4492A0B8-068F-4002-9E8D-E1F5FED367F0}" name="Category" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{47C54592-75B0-4C70-BBF8-0F40483670E9}" name="Progress" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{663FB5E0-7616-4EA5-B56A-FF069E2E07D7}" name="Start" dataDxfId="15" dataCellStyle="Date">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3B766962-C06F-4E12-BE91-12AB93439874}" name="Days" dataDxfId="0" dataCellStyle="Comma [0]"/>
+    <tableColumn id="6" xr3:uid="{3B766962-C06F-4E12-BE91-12AB93439874}" name="Days" dataDxfId="14" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="ToDoList" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2391,8 +2391,8 @@
   </sheetPr>
   <dimension ref="A1:BO109"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A17" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3192,7 +3192,7 @@
       <c r="D10" s="46"/>
       <c r="E10" s="85">
         <f t="shared" ref="E10:E108" ca="1" si="4">TODAY()</f>
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="F10" s="47"/>
       <c r="H10" s="48"/>
@@ -7858,7 +7858,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
       <c r="B30" s="56" t="s">
         <v>48</v>
@@ -7867,7 +7867,7 @@
         <v>10</v>
       </c>
       <c r="D30" s="57">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E30" s="87">
         <v>45363</v>
@@ -8101,7 +8101,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="56" t="s">
         <v>49</v>
@@ -8110,7 +8110,7 @@
         <v>10</v>
       </c>
       <c r="D31" s="57">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E31" s="87">
         <v>45364</v>
@@ -8344,7 +8344,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
       <c r="B32" s="56" t="s">
         <v>43</v>
@@ -8353,7 +8353,7 @@
         <v>10</v>
       </c>
       <c r="D32" s="57">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E32" s="87">
         <v>45362</v>
@@ -8587,7 +8587,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" s="56" t="s">
         <v>38</v>
@@ -8596,7 +8596,7 @@
         <v>10</v>
       </c>
       <c r="D33" s="57">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E33" s="87">
         <v>45363</v>
@@ -9082,7 +9082,7 @@
         <v>10</v>
       </c>
       <c r="D35" s="57">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E35" s="87">
         <v>45370</v>
@@ -9325,7 +9325,7 @@
         <v>10</v>
       </c>
       <c r="D36" s="57">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E36" s="87">
         <v>45371</v>
@@ -9568,7 +9568,7 @@
         <v>10</v>
       </c>
       <c r="D37" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" s="87">
         <v>45369</v>
@@ -9811,7 +9811,7 @@
         <v>10</v>
       </c>
       <c r="D38" s="57">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E38" s="87">
         <v>45370</v>
@@ -23596,7 +23596,7 @@
       <c r="D95" s="68"/>
       <c r="E95" s="90">
         <f t="shared" ca="1" si="4"/>
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="F95" s="69"/>
       <c r="G95" s="53"/>
@@ -23836,7 +23836,7 @@
       </c>
       <c r="E96" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="F96" s="58">
         <v>4</v>
@@ -24078,7 +24078,7 @@
       </c>
       <c r="E97" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="F97" s="58">
         <v>14</v>
@@ -24320,7 +24320,7 @@
       </c>
       <c r="E98" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="F98" s="58">
         <v>6</v>
@@ -24562,7 +24562,7 @@
       </c>
       <c r="E99" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="F99" s="58">
         <v>3</v>
@@ -24804,7 +24804,7 @@
       </c>
       <c r="E100" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="F100" s="58">
         <v>19</v>
@@ -25044,7 +25044,7 @@
       <c r="D101" s="72"/>
       <c r="E101" s="91">
         <f t="shared" ca="1" si="4"/>
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="F101" s="73"/>
       <c r="G101" s="53"/>
@@ -25284,7 +25284,7 @@
       </c>
       <c r="E102" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="F102" s="58">
         <v>15</v>
@@ -25526,7 +25526,7 @@
       </c>
       <c r="E103" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="F103" s="58">
         <v>5</v>
@@ -25768,7 +25768,7 @@
       </c>
       <c r="E104" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="F104" s="58">
         <v>1</v>
@@ -26010,7 +26010,7 @@
       </c>
       <c r="E105" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="F105" s="58"/>
       <c r="G105" s="53"/>
@@ -26250,7 +26250,7 @@
       </c>
       <c r="E106" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="F106" s="58"/>
       <c r="G106" s="53"/>
@@ -26486,7 +26486,7 @@
       <c r="D107" s="57"/>
       <c r="E107" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="F107" s="58"/>
       <c r="G107" s="53"/>
@@ -26725,7 +26725,7 @@
       <c r="D108" s="21"/>
       <c r="E108" s="92">
         <f t="shared" ca="1" si="4"/>
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="F108" s="76"/>
       <c r="G108" s="53"/>
@@ -26816,58 +26816,58 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H6:AL6">
+    <cfRule type="expression" dxfId="13" priority="4">
+      <formula>H$7&lt;=EOMONTH($H$7,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:BK6">
+    <cfRule type="expression" dxfId="12" priority="2">
+      <formula>AND(H$7&lt;=EOMONTH($H$7,1),H$7&gt;EOMONTH($H$7,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H7:BK108">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>AND(TODAY()&gt;=H$7,TODAY()&lt;I$7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:AL6">
-    <cfRule type="expression" dxfId="19" priority="4">
-      <formula>H$7&lt;=EOMONTH($H$7,0)</formula>
+  <conditionalFormatting sqref="H10:BK107">
+    <cfRule type="expression" dxfId="10" priority="18" stopIfTrue="1">
+      <formula>AND($C10="Low Risk",H$7&gt;=$E10,H$7&lt;=$E10+$F10-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="19" stopIfTrue="1">
+      <formula>AND($C10="High Risk",H$7&gt;=$E10,H$7&lt;=$E10+$F10-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="20" stopIfTrue="1">
+      <formula>AND($C10="On Track",H$7&gt;=$E10,H$7&lt;=$E10+$F10-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="21" stopIfTrue="1">
+      <formula>AND($C10="Med Risk",H$7&gt;=$E10,H$7&lt;=$E10+$F10-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="22" stopIfTrue="1">
+      <formula>AND(LEN($C10)=0,H$7&gt;=$E10,H$7&lt;=$E10+$F10-1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H108:BK108">
+    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
+      <formula>AND(#REF!="Low Risk",H$7&gt;=#REF!,H$7&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="14" stopIfTrue="1">
+      <formula>AND(#REF!="High Risk",H$7&gt;=#REF!,H$7&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="15" stopIfTrue="1">
+      <formula>AND(#REF!="On Track",H$7&gt;=#REF!,H$7&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="16" stopIfTrue="1">
+      <formula>AND(#REF!="Med Risk",H$7&gt;=#REF!,H$7&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="17" stopIfTrue="1">
+      <formula>AND(LEN(#REF!)=0,H$7&gt;=#REF!,H$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BK6">
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>AND(I$7&lt;=EOMONTH($H$7,2),I$7&gt;EOMONTH($H$7,0),I$7&gt;EOMONTH($H$7,1))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6:BK6">
-    <cfRule type="expression" dxfId="17" priority="2">
-      <formula>AND(H$7&lt;=EOMONTH($H$7,1),H$7&gt;EOMONTH($H$7,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H108:BK108">
-    <cfRule type="expression" dxfId="16" priority="13" stopIfTrue="1">
-      <formula>AND(#REF!="Low Risk",H$7&gt;=#REF!,H$7&lt;=#REF!+#REF!-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="14" stopIfTrue="1">
-      <formula>AND(#REF!="High Risk",H$7&gt;=#REF!,H$7&lt;=#REF!+#REF!-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
-      <formula>AND(#REF!="On Track",H$7&gt;=#REF!,H$7&lt;=#REF!+#REF!-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="16" stopIfTrue="1">
-      <formula>AND(#REF!="Med Risk",H$7&gt;=#REF!,H$7&lt;=#REF!+#REF!-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="17" stopIfTrue="1">
-      <formula>AND(LEN(#REF!)=0,H$7&gt;=#REF!,H$7&lt;=#REF!+#REF!-1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10:BK107">
-    <cfRule type="expression" dxfId="11" priority="18" stopIfTrue="1">
-      <formula>AND($C10="Low Risk",H$7&gt;=$E10,H$7&lt;=$E10+$F10-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="19" stopIfTrue="1">
-      <formula>AND($C10="High Risk",H$7&gt;=$E10,H$7&lt;=$E10+$F10-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="20" stopIfTrue="1">
-      <formula>AND($C10="On Track",H$7&gt;=$E10,H$7&lt;=$E10+$F10-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="21" stopIfTrue="1">
-      <formula>AND($C10="Med Risk",H$7&gt;=$E10,H$7&lt;=$E10+$F10-1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="22" stopIfTrue="1">
-      <formula>AND(LEN($C10)=0,H$7&gt;=$E10,H$7&lt;=$E10+$F10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="13">
@@ -26949,6 +26949,25 @@
           <xm:sqref>D9:D108</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="72" id="{67763332-2AE9-4F93-8BB7-5ECDB6B99BA2}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H10:BK107</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="12" id="{5AD67FB9-23B4-4F54-BD80-7A6CF9720346}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -26966,25 +26985,6 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>H108:BK108</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="72" id="{67763332-2AE9-4F93-8BB7-5ECDB6B99BA2}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>H10:BK107</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -27182,6 +27182,26 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -27481,26 +27501,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16A2ABA2-2AE7-458F-84A6-54746C92ACFB}">
   <ds:schemaRefs>
@@ -27510,6 +27510,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D0FD509-FAA6-490F-8E99-57602ADB216E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CDF409-87B8-4BD3-A7A0-FA31B09DB512}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27530,18 +27542,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D0FD509-FAA6-490F-8E99-57602ADB216E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
conditions finished && feats TODO styling && started races && started researching entity api for node creation in Drupal
</commit_message>
<xml_diff>
--- a/Intern Documentation/DnDUnderground Planning.xlsx
+++ b/Intern Documentation/DnDUnderground Planning.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68502489-BB86-49FF-85BF-3777057693BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BC6315-E539-471A-A219-97E823572A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2391,8 +2391,8 @@
   </sheetPr>
   <dimension ref="A1:BO109"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A24" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="X56" sqref="X56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3192,7 +3192,7 @@
       <c r="D10" s="46"/>
       <c r="E10" s="85">
         <f t="shared" ref="E10:E108" ca="1" si="4">TODAY()</f>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="F10" s="47"/>
       <c r="H10" s="48"/>
@@ -5194,7 +5194,7 @@
         <v>6</v>
       </c>
       <c r="D19" s="72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="98">
         <v>45348</v>
@@ -6409,7 +6409,7 @@
         <v>6</v>
       </c>
       <c r="D24" s="72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="98">
         <v>45355</v>
@@ -7624,7 +7624,7 @@
         <v>6</v>
       </c>
       <c r="D29" s="72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="98">
         <v>45362</v>
@@ -8839,7 +8839,7 @@
         <v>6</v>
       </c>
       <c r="D34" s="72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="98">
         <v>45369</v>
@@ -9073,7 +9073,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11"/>
       <c r="B35" s="56" t="s">
         <v>50</v>
@@ -9082,7 +9082,7 @@
         <v>10</v>
       </c>
       <c r="D35" s="57">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E35" s="87">
         <v>45370</v>
@@ -9316,7 +9316,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
       <c r="B36" s="56" t="s">
         <v>51</v>
@@ -9325,7 +9325,7 @@
         <v>10</v>
       </c>
       <c r="D36" s="57">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E36" s="87">
         <v>45371</v>
@@ -9559,7 +9559,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11"/>
       <c r="B37" s="56" t="s">
         <v>43</v>
@@ -9802,7 +9802,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:63" s="18" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:63" s="18" customFormat="1" ht="39.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11"/>
       <c r="B38" s="56" t="s">
         <v>38</v>
@@ -9811,7 +9811,7 @@
         <v>10</v>
       </c>
       <c r="D38" s="57">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E38" s="87">
         <v>45370</v>
@@ -10054,7 +10054,7 @@
         <v>6</v>
       </c>
       <c r="D39" s="72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="98">
         <v>45376</v>
@@ -11269,7 +11269,7 @@
         <v>6</v>
       </c>
       <c r="D44" s="72">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="E44" s="98">
         <v>45383</v>
@@ -11512,7 +11512,7 @@
         <v>10</v>
       </c>
       <c r="D45" s="57">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="E45" s="87">
         <v>45384</v>
@@ -11755,7 +11755,7 @@
         <v>10</v>
       </c>
       <c r="D46" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" s="87">
         <v>45383</v>
@@ -11998,7 +11998,7 @@
         <v>10</v>
       </c>
       <c r="D47" s="57">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="E47" s="87">
         <v>45384</v>
@@ -12241,7 +12241,7 @@
         <v>6</v>
       </c>
       <c r="D48" s="72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="98">
         <v>45390</v>
@@ -12475,7 +12475,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11"/>
       <c r="B49" s="56" t="s">
         <v>58</v>
@@ -12484,7 +12484,7 @@
         <v>10</v>
       </c>
       <c r="D49" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" s="87">
         <v>45391</v>
@@ -12718,7 +12718,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11"/>
       <c r="B50" s="56" t="s">
         <v>43</v>
@@ -12727,7 +12727,7 @@
         <v>10</v>
       </c>
       <c r="D50" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" s="87">
         <v>45390</v>
@@ -12961,7 +12961,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:63" s="18" customFormat="1" ht="40.049999999999997" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11"/>
       <c r="B51" s="56" t="s">
         <v>38</v>
@@ -12970,7 +12970,7 @@
         <v>10</v>
       </c>
       <c r="D51" s="57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51" s="87">
         <v>45391</v>
@@ -23596,7 +23596,7 @@
       <c r="D95" s="68"/>
       <c r="E95" s="90">
         <f t="shared" ca="1" si="4"/>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="F95" s="69"/>
       <c r="G95" s="53"/>
@@ -23836,7 +23836,7 @@
       </c>
       <c r="E96" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="F96" s="58">
         <v>4</v>
@@ -24078,7 +24078,7 @@
       </c>
       <c r="E97" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="F97" s="58">
         <v>14</v>
@@ -24320,7 +24320,7 @@
       </c>
       <c r="E98" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="F98" s="58">
         <v>6</v>
@@ -24562,7 +24562,7 @@
       </c>
       <c r="E99" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="F99" s="58">
         <v>3</v>
@@ -24804,7 +24804,7 @@
       </c>
       <c r="E100" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="F100" s="58">
         <v>19</v>
@@ -25044,7 +25044,7 @@
       <c r="D101" s="72"/>
       <c r="E101" s="91">
         <f t="shared" ca="1" si="4"/>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="F101" s="73"/>
       <c r="G101" s="53"/>
@@ -25284,7 +25284,7 @@
       </c>
       <c r="E102" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="F102" s="58">
         <v>15</v>
@@ -25526,7 +25526,7 @@
       </c>
       <c r="E103" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="F103" s="58">
         <v>5</v>
@@ -25768,7 +25768,7 @@
       </c>
       <c r="E104" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="F104" s="58">
         <v>1</v>
@@ -26010,7 +26010,7 @@
       </c>
       <c r="E105" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="F105" s="58"/>
       <c r="G105" s="53"/>
@@ -26250,7 +26250,7 @@
       </c>
       <c r="E106" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="F106" s="58"/>
       <c r="G106" s="53"/>
@@ -26486,7 +26486,7 @@
       <c r="D107" s="57"/>
       <c r="E107" s="87">
         <f t="shared" ca="1" si="4"/>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="F107" s="58"/>
       <c r="G107" s="53"/>
@@ -26725,7 +26725,7 @@
       <c r="D108" s="21"/>
       <c r="E108" s="92">
         <f t="shared" ca="1" si="4"/>
-        <v>45365</v>
+        <v>45371</v>
       </c>
       <c r="F108" s="76"/>
       <c r="G108" s="53"/>
@@ -27182,26 +27182,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -27501,6 +27481,26 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16A2ABA2-2AE7-458F-84A6-54746C92ACFB}">
   <ds:schemaRefs>
@@ -27510,18 +27510,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D0FD509-FAA6-490F-8E99-57602ADB216E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CDF409-87B8-4BD3-A7A0-FA31B09DB512}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27542,6 +27530,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D0FD509-FAA6-490F-8E99-57602ADB216E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>